<commit_message>
Did some edits and added more marks
</commit_message>
<xml_diff>
--- a/Resources/IMDb_Top_250_TV_Shows.xlsx
+++ b/Resources/IMDb_Top_250_TV_Shows.xlsx
@@ -2057,12 +2057,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Rome</t>
+          <t>Kota Factory</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2079,12 +2079,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Kota Factory</t>
+          <t>Rome</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -3025,12 +3025,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Daredevil</t>
+          <t>Demon Slayer: Kimetsu no Yaiba</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3047,12 +3047,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Demon Slayer: Kimetsu no Yaiba</t>
+          <t>Daredevil</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3091,12 +3091,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Young Justice</t>
+          <t>Haikyuu!!</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3113,12 +3113,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Haikyuu!!</t>
+          <t>Young Justice</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3993,12 +3993,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Crash Landing on You</t>
+          <t>Jujutsu Kaisen</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -4015,12 +4015,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Jujutsu Kaisen</t>
+          <t>Crash Landing on You</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -4169,12 +4169,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Coupling</t>
+          <t>Mahabharat</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>1988</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -4191,12 +4191,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Mahabharat</t>
+          <t>Coupling</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>1988</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -4367,12 +4367,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Louie</t>
+          <t>Gullak</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -4389,12 +4389,12 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Gullak</t>
+          <t>Louie</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -4983,12 +4983,12 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Rurouni Kenshin: Trust and Betrayal</t>
+          <t>Detectorists</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>1999</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
@@ -5005,12 +5005,12 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Detectorists</t>
+          <t>Rurouni Kenshin: Trust and Betrayal</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
@@ -5401,12 +5401,12 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>John Adams</t>
+          <t>Erased</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>2008</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
@@ -5423,12 +5423,12 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Erased</t>
+          <t>John Adams</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2008</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
@@ -5731,12 +5731,12 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Your Lie in April</t>
+          <t>I Love Lucy</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>1951</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -5753,12 +5753,12 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>I Love Lucy</t>
+          <t>Your Lie in April</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>1951</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -5929,12 +5929,12 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Clannad: After Story</t>
+          <t>Avrupa Yakasi</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>2008</t>
+          <t>2004</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">

</xml_diff>